<commit_message>
removed updated info from appredict version info
</commit_message>
<xml_diff>
--- a/client/simulations/tests/all_data.xlsx
+++ b/client/simulations/tests/all_data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uczmh2\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uczmh2\Desktop\ap-nimbus-client\client\simulations\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="11700"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="11700" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Input Values" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="97">
   <si>
     <t>Title</t>
   </si>
@@ -237,12 +237,6 @@
   </si>
   <si>
     <t>2019.1.682dce0</t>
-  </si>
-  <si>
-    <t>Modified</t>
-  </si>
-  <si>
-    <t>True</t>
   </si>
   <si>
     <t>Build options</t>
@@ -673,7 +667,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -69703,10 +69697,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -69831,14 +69825,6 @@
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>97</v>
-      </c>
-      <c r="B16" t="s">
-        <v>98</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>